<commit_message>
thay doi nhan excel nguoi lao dong
</commit_message>
<xml_diff>
--- a/public/huongdan.xlsx
+++ b/public/huongdan.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tailieu\PM QLVL\quanlyvieclam\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC9B17A-5963-444E-8336-C989D70DDD40}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" forceFullCalc="1"/>
+  <calcPr calcId="179021" forceFullCalc="1"/>
 </workbook>
 </file>
 
@@ -243,9 +244,6 @@
     <t>0 nếu sai hoặc 1 nếu đúng</t>
   </si>
   <si>
-    <t>Định dạng Date của Excel (vd: 31/12/1990), nếu đúng nó tự động căn phải trong Ô.</t>
-  </si>
-  <si>
     <t>Ví dụ : Bảo Ninh</t>
   </si>
   <si>
@@ -274,12 +272,15 @@
   </si>
   <si>
     <t>Định dạng text</t>
+  </si>
+  <si>
+    <t>Định dạng text. Ghi theo mẫu: dd/mm/yyyy (vd:01/01/2023)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -428,6 +429,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -463,6 +481,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -638,11 +673,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,7 +690,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>34</v>
@@ -680,7 +715,7 @@
         <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -691,7 +726,7 @@
         <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -702,7 +737,7 @@
         <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -721,7 +756,7 @@
         <v>41</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -754,7 +789,7 @@
         <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -773,7 +808,7 @@
         <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -784,7 +819,7 @@
         <v>49</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -795,7 +830,7 @@
         <v>50</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -806,7 +841,7 @@
         <v>51</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -817,7 +852,7 @@
         <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -828,7 +863,7 @@
         <v>53</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -839,7 +874,7 @@
         <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -850,7 +885,7 @@
         <v>55</v>
       </c>
       <c r="C19" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -909,7 +944,7 @@
         <v>62</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -920,7 +955,7 @@
         <v>63</v>
       </c>
       <c r="C27" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -947,7 +982,7 @@
         <v>66</v>
       </c>
       <c r="C30" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -958,7 +993,7 @@
         <v>67</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix lai huongdan excel nhap nguoi lao dong doanh nghiep
</commit_message>
<xml_diff>
--- a/public/huongdan.xlsx
+++ b/public/huongdan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tailieu\PM QLVL\quanlyvieclam\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC9B17A-5963-444E-8336-C989D70DDD40}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A78B001-2C1A-4281-B4ED-04A4DEDC9FA6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="86">
   <si>
     <t>hoten</t>
   </si>
@@ -275,6 +275,9 @@
   </si>
   <si>
     <t>Định dạng text. Ghi theo mẫu: dd/mm/yyyy (vd:01/01/2023)</t>
+  </si>
+  <si>
+    <t>Định dạng text.Nếu có số 0 ở đầu tiên thì ghi theo vd: '042094014612</t>
   </si>
 </sst>
 </file>
@@ -676,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,7 +740,7 @@
         <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>